<commit_message>
add soft_bottom to hab_trend_gye2015 layer
</commit_message>
<xml_diff>
--- a/region2015/pre-proc/hab_trend_2/Respaldos Habitat destruction subtidal soft bottom-1.xlsx
+++ b/region2015/pre-proc/hab_trend_2/Respaldos Habitat destruction subtidal soft bottom-1.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Local" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="final" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
   <si>
     <t>dredges</t>
   </si>
@@ -27,7 +28,7 @@
     <t>bottom trawls</t>
   </si>
   <si>
-    <t>shrimp trawls (mid-water trawls were excluded).  </t>
+    <t>shrimp trawls (mid-water trawls were excluded).</t>
   </si>
   <si>
     <t>Capturas</t>
@@ -51,7 +52,7 @@
     <t>Mediana</t>
   </si>
   <si>
-    <t>Presión </t>
+    <t>Presión</t>
   </si>
   <si>
     <t>Year</t>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>Noreste Isla Puná y Sur canal de Jambelí</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -345,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -526,14 +530,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -635,15 +631,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>38880</xdr:colOff>
+      <xdr:colOff>65880</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>133920</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -658,8 +654,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7150680" y="12556800"/>
-          <a:ext cx="9239040" cy="3895200"/>
+          <a:off x="7177680" y="12547800"/>
+          <a:ext cx="9238680" cy="3894840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -674,15 +670,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>536040</xdr:colOff>
+      <xdr:colOff>563040</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
+      <xdr:colOff>714600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -691,8 +687,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9680040" y="212760"/>
-          <a:ext cx="8279640" cy="628200"/>
+          <a:off x="9707040" y="203760"/>
+          <a:ext cx="8279280" cy="627840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -728,15 +724,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>562680</xdr:colOff>
+      <xdr:colOff>589680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>638280</xdr:colOff>
+      <xdr:colOff>664920</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -751,8 +747,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="42218640" y="1781280"/>
-          <a:ext cx="4139640" cy="4618800"/>
+          <a:off x="42245640" y="1772280"/>
+          <a:ext cx="4139280" cy="4618440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,15 +768,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>269640</xdr:colOff>
+      <xdr:colOff>296640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>433080</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:colOff>459720</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -795,8 +791,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="31765320" y="829080"/>
-          <a:ext cx="3211560" cy="3619080"/>
+          <a:off x="31792320" y="820080"/>
+          <a:ext cx="3211200" cy="3618720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8131,14 +8127,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AC49"/>
+  <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8146,6 +8142,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.4251012145749"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>0</v>
@@ -8208,7 +8205,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
@@ -8389,7 +8386,7 @@
       </c>
       <c r="Z8" s="42" t="n">
         <f aca="false">+MEDIAN(W8:W22)</f>
-        <v>0.236247408664741</v>
+        <v>0.236247408664742</v>
       </c>
       <c r="AA8" s="43" t="n">
         <f aca="false">1-X8</f>
@@ -8401,7 +8398,7 @@
       </c>
       <c r="AC8" s="43" t="n">
         <f aca="false">1-Z8</f>
-        <v>0.763752591335259</v>
+        <v>0.763752591335258</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8419,15 +8416,15 @@
       </c>
       <c r="F9" s="36" t="n">
         <f aca="false">$E9/3</f>
-        <v>826.333333333334</v>
+        <v>826.333333333333</v>
       </c>
       <c r="G9" s="36" t="n">
         <f aca="false">$E9/3</f>
-        <v>826.333333333334</v>
+        <v>826.333333333333</v>
       </c>
       <c r="H9" s="36" t="n">
         <f aca="false">$E9/3</f>
-        <v>826.333333333334</v>
+        <v>826.333333333333</v>
       </c>
       <c r="I9" s="40" t="n">
         <f aca="false">+I8</f>
@@ -8455,7 +8452,7 @@
       </c>
       <c r="O9" s="36" t="n">
         <f aca="false">+LOG(L9+1)</f>
-        <v>0.0736710661216454</v>
+        <v>0.0736710661216453</v>
       </c>
       <c r="P9" s="36" t="n">
         <f aca="false">+LOG(M9+1)</f>
@@ -8479,7 +8476,7 @@
       </c>
       <c r="U9" s="41" t="n">
         <f aca="false">1-R9</f>
-        <v>0.802442978270216</v>
+        <v>0.802442978270217</v>
       </c>
       <c r="V9" s="41" t="n">
         <f aca="false">1-S9</f>
@@ -8591,15 +8588,15 @@
       </c>
       <c r="F11" s="36" t="n">
         <f aca="false">$E11/3</f>
-        <v>847.933333333333</v>
+        <v>847.933333333334</v>
       </c>
       <c r="G11" s="36" t="n">
         <f aca="false">$E11/3</f>
-        <v>847.933333333333</v>
+        <v>847.933333333334</v>
       </c>
       <c r="H11" s="36" t="n">
         <f aca="false">$E11/3</f>
-        <v>847.933333333333</v>
+        <v>847.933333333334</v>
       </c>
       <c r="I11" s="40" t="n">
         <f aca="false">+I10</f>
@@ -8619,11 +8616,11 @@
       </c>
       <c r="M11" s="36" t="n">
         <f aca="false">+G11/J11</f>
-        <v>0.135238211226434</v>
+        <v>0.135238211226435</v>
       </c>
       <c r="N11" s="36" t="n">
         <f aca="false">+H11/K11</f>
-        <v>0.646172054194118</v>
+        <v>0.646172054194119</v>
       </c>
       <c r="O11" s="36" t="n">
         <f aca="false">+LOG(L11+1)</f>
@@ -8789,11 +8786,11 @@
       </c>
       <c r="L13" s="36" t="n">
         <f aca="false">+F13/I13</f>
-        <v>1.00797080056348</v>
+        <v>1.00797080056347</v>
       </c>
       <c r="M13" s="36" t="n">
         <f aca="false">+G13/J13</f>
-        <v>0.718575107245248</v>
+        <v>0.718575107245247</v>
       </c>
       <c r="N13" s="36" t="n">
         <f aca="false">+H13/K13</f>
@@ -8801,7 +8798,7 @@
       </c>
       <c r="O13" s="36" t="n">
         <f aca="false">+LOG(L13+1)</f>
-        <v>0.302757393111249</v>
+        <v>0.302757393111248</v>
       </c>
       <c r="P13" s="36" t="n">
         <f aca="false">+LOG(M13+1)</f>
@@ -8813,15 +8810,15 @@
       </c>
       <c r="R13" s="36" t="n">
         <f aca="false">+O13*1/MAX($O$8:$O$22)</f>
-        <v>0.811877064341249</v>
+        <v>0.811877064341248</v>
       </c>
       <c r="S13" s="36" t="n">
         <f aca="false">+P13*1/MAX($P$8:$P$22)</f>
-        <v>0.79890882975606</v>
+        <v>0.798908829756059</v>
       </c>
       <c r="T13" s="36" t="n">
         <f aca="false">+Q13*1/MAX($Q$8:$Q$22)</f>
-        <v>0.861512833939218</v>
+        <v>0.861512833939217</v>
       </c>
       <c r="U13" s="41" t="n">
         <f aca="false">1-R13</f>
@@ -8829,11 +8826,11 @@
       </c>
       <c r="V13" s="41" t="n">
         <f aca="false">1-S13</f>
-        <v>0.20109117024394</v>
+        <v>0.201091170243941</v>
       </c>
       <c r="W13" s="41" t="n">
         <f aca="false">1-T13</f>
-        <v>0.138487166060782</v>
+        <v>0.138487166060783</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8885,7 +8882,7 @@
       </c>
       <c r="N14" s="36" t="n">
         <f aca="false">+H14/K14</f>
-        <v>2.25665010775897</v>
+        <v>2.25665010775896</v>
       </c>
       <c r="O14" s="36" t="n">
         <f aca="false">+LOG(L14+1)</f>
@@ -9205,27 +9202,27 @@
         <f aca="false">+B18+C18+D18</f>
         <v>18236.6</v>
       </c>
-      <c r="F18" s="45" t="n">
+      <c r="F18" s="36" t="n">
         <f aca="false">$E18/3</f>
         <v>6078.86666666667</v>
       </c>
-      <c r="G18" s="45" t="n">
+      <c r="G18" s="36" t="n">
         <f aca="false">$E18/3</f>
         <v>6078.86666666667</v>
       </c>
-      <c r="H18" s="45" t="n">
+      <c r="H18" s="36" t="n">
         <f aca="false">$E18/3</f>
         <v>6078.86666666667</v>
       </c>
-      <c r="I18" s="46" t="n">
+      <c r="I18" s="40" t="n">
         <f aca="false">+I17</f>
         <v>4469.7837</v>
       </c>
-      <c r="J18" s="46" t="n">
+      <c r="J18" s="40" t="n">
         <f aca="false">+J17</f>
         <v>6269.9242</v>
       </c>
-      <c r="K18" s="46" t="n">
+      <c r="K18" s="40" t="n">
         <f aca="false">+K17</f>
         <v>1312.2408</v>
       </c>
@@ -9295,27 +9292,27 @@
         <f aca="false">+B19+C19+D19</f>
         <v>12393</v>
       </c>
-      <c r="F19" s="45" t="n">
+      <c r="F19" s="36" t="n">
         <f aca="false">$E19/3</f>
         <v>4131</v>
       </c>
-      <c r="G19" s="45" t="n">
+      <c r="G19" s="36" t="n">
         <f aca="false">$E19/3</f>
         <v>4131</v>
       </c>
-      <c r="H19" s="45" t="n">
+      <c r="H19" s="36" t="n">
         <f aca="false">$E19/3</f>
         <v>4131</v>
       </c>
-      <c r="I19" s="46" t="n">
+      <c r="I19" s="40" t="n">
         <f aca="false">+I18</f>
         <v>4469.7837</v>
       </c>
-      <c r="J19" s="46" t="n">
+      <c r="J19" s="40" t="n">
         <f aca="false">+J18</f>
         <v>6269.9242</v>
       </c>
-      <c r="K19" s="46" t="n">
+      <c r="K19" s="40" t="n">
         <f aca="false">+K18</f>
         <v>1312.2408</v>
       </c>
@@ -9385,27 +9382,27 @@
         <f aca="false">+B20+C20+D20</f>
         <v>14680.2</v>
       </c>
-      <c r="F20" s="45" t="n">
+      <c r="F20" s="36" t="n">
         <f aca="false">$E20/3</f>
         <v>4893.4</v>
       </c>
-      <c r="G20" s="45" t="n">
+      <c r="G20" s="36" t="n">
         <f aca="false">$E20/3</f>
         <v>4893.4</v>
       </c>
-      <c r="H20" s="45" t="n">
+      <c r="H20" s="36" t="n">
         <f aca="false">$E20/3</f>
         <v>4893.4</v>
       </c>
-      <c r="I20" s="46" t="n">
+      <c r="I20" s="40" t="n">
         <f aca="false">+I19</f>
         <v>4469.7837</v>
       </c>
-      <c r="J20" s="46" t="n">
+      <c r="J20" s="40" t="n">
         <f aca="false">+J19</f>
         <v>6269.9242</v>
       </c>
-      <c r="K20" s="46" t="n">
+      <c r="K20" s="40" t="n">
         <f aca="false">+K19</f>
         <v>1312.2408</v>
       </c>
@@ -9475,27 +9472,27 @@
         <f aca="false">+B21+C21+D21</f>
         <v>10802.7110866363</v>
       </c>
-      <c r="F21" s="45" t="n">
+      <c r="F21" s="36" t="n">
         <f aca="false">$E21/3</f>
         <v>3600.90369554544</v>
       </c>
-      <c r="G21" s="45" t="n">
+      <c r="G21" s="36" t="n">
         <f aca="false">$E21/3</f>
         <v>3600.90369554544</v>
       </c>
-      <c r="H21" s="45" t="n">
+      <c r="H21" s="36" t="n">
         <f aca="false">$E21/3</f>
         <v>3600.90369554544</v>
       </c>
-      <c r="I21" s="46" t="n">
+      <c r="I21" s="40" t="n">
         <f aca="false">+I20</f>
         <v>4469.7837</v>
       </c>
-      <c r="J21" s="46" t="n">
+      <c r="J21" s="40" t="n">
         <f aca="false">+J20</f>
         <v>6269.9242</v>
       </c>
-      <c r="K21" s="46" t="n">
+      <c r="K21" s="40" t="n">
         <f aca="false">+K20</f>
         <v>1312.2408</v>
       </c>
@@ -9533,7 +9530,7 @@
       </c>
       <c r="T21" s="36" t="n">
         <f aca="false">+Q21*1/MAX($Q$8:$Q$22)</f>
-        <v>0.763752591335259</v>
+        <v>0.763752591335258</v>
       </c>
       <c r="U21" s="41" t="n">
         <f aca="false">1-R21</f>
@@ -9545,7 +9542,7 @@
       </c>
       <c r="W21" s="41" t="n">
         <f aca="false">1-T21</f>
-        <v>0.236247408664741</v>
+        <v>0.236247408664742</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9561,27 +9558,27 @@
         <f aca="false">+B22+C22+D22</f>
         <v>3019</v>
       </c>
-      <c r="F22" s="45" t="n">
+      <c r="F22" s="36" t="n">
         <f aca="false">$E22/3</f>
         <v>1006.33333333333</v>
       </c>
-      <c r="G22" s="45" t="n">
+      <c r="G22" s="36" t="n">
         <f aca="false">$E22/3</f>
         <v>1006.33333333333</v>
       </c>
-      <c r="H22" s="45" t="n">
+      <c r="H22" s="36" t="n">
         <f aca="false">$E22/3</f>
         <v>1006.33333333333</v>
       </c>
-      <c r="I22" s="46" t="n">
+      <c r="I22" s="40" t="n">
         <f aca="false">+I21</f>
         <v>4469.7837</v>
       </c>
-      <c r="J22" s="46" t="n">
+      <c r="J22" s="40" t="n">
         <f aca="false">+J21</f>
         <v>6269.9242</v>
       </c>
-      <c r="K22" s="46" t="n">
+      <c r="K22" s="40" t="n">
         <f aca="false">+K21</f>
         <v>1312.2408</v>
       </c>
@@ -9643,7 +9640,7 @@
       <c r="H35" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="47" t="s">
+      <c r="L35" s="45" t="s">
         <v>32</v>
       </c>
       <c r="O35" s="0" t="s">
@@ -9651,22 +9648,22 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="48" t="s">
+      <c r="F36" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="48" t="s">
+      <c r="G36" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="49" t="s">
+      <c r="I36" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="K36" s="50" t="n">
+      <c r="K36" s="48" t="n">
         <v>2005</v>
       </c>
-      <c r="L36" s="51" t="n">
+      <c r="L36" s="49" t="n">
         <v>11154.7343633037</v>
       </c>
       <c r="N36" s="0" t="n">
@@ -9687,13 +9684,13 @@
         <f aca="false">+G37/2200</f>
         <v>4017.6</v>
       </c>
-      <c r="I37" s="52" t="s">
+      <c r="I37" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="50" t="n">
+      <c r="K37" s="48" t="n">
         <v>2006</v>
       </c>
-      <c r="L37" s="51" t="n">
+      <c r="L37" s="49" t="n">
         <v>6395.70502817713</v>
       </c>
       <c r="N37" s="0" t="n">
@@ -9714,11 +9711,11 @@
         <f aca="false">+G38/2200</f>
         <v>4017.6</v>
       </c>
-      <c r="I38" s="52"/>
-      <c r="K38" s="50" t="n">
+      <c r="I38" s="50"/>
+      <c r="K38" s="48" t="n">
         <v>2007</v>
       </c>
-      <c r="L38" s="51" t="n">
+      <c r="L38" s="49" t="n">
         <v>5900</v>
       </c>
       <c r="N38" s="0" t="n">
@@ -9739,11 +9736,11 @@
         <f aca="false">+G39/2200</f>
         <v>3542.4</v>
       </c>
-      <c r="I39" s="52"/>
-      <c r="K39" s="50" t="n">
+      <c r="I39" s="50"/>
+      <c r="K39" s="48" t="n">
         <v>2008</v>
       </c>
-      <c r="L39" s="51" t="n">
+      <c r="L39" s="49" t="n">
         <v>5704</v>
       </c>
       <c r="N39" s="0" t="n">
@@ -9764,11 +9761,11 @@
         <f aca="false">+G40/2200</f>
         <v>1771.2</v>
       </c>
-      <c r="I40" s="52"/>
-      <c r="K40" s="50" t="n">
+      <c r="I40" s="50"/>
+      <c r="K40" s="48" t="n">
         <v>2009</v>
       </c>
-      <c r="L40" s="51" t="n">
+      <c r="L40" s="49" t="n">
         <v>7011.93645687646</v>
       </c>
       <c r="N40" s="0" t="n">
@@ -9779,10 +9776,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K41" s="50" t="n">
+      <c r="K41" s="48" t="n">
         <v>2010</v>
       </c>
-      <c r="L41" s="51" t="n">
+      <c r="L41" s="49" t="n">
         <v>7155</v>
       </c>
       <c r="N41" s="0" t="n">
@@ -9793,10 +9790,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K42" s="50" t="n">
+      <c r="K42" s="48" t="n">
         <v>2011</v>
       </c>
-      <c r="L42" s="51" t="n">
+      <c r="L42" s="49" t="n">
         <v>4187.7</v>
       </c>
       <c r="N42" s="0" t="n">
@@ -9807,10 +9804,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K43" s="50" t="n">
+      <c r="K43" s="48" t="n">
         <v>2012</v>
       </c>
-      <c r="L43" s="51" t="n">
+      <c r="L43" s="49" t="n">
         <v>5568.9</v>
       </c>
       <c r="N43" s="0" t="n">
@@ -9821,10 +9818,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K44" s="50" t="n">
+      <c r="K44" s="48" t="n">
         <v>2013</v>
       </c>
-      <c r="L44" s="51" t="n">
+      <c r="L44" s="49" t="n">
         <v>2074</v>
       </c>
       <c r="N44" s="0" t="n">
@@ -9835,10 +9832,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K45" s="50" t="n">
+      <c r="K45" s="48" t="n">
         <v>2014</v>
       </c>
-      <c r="L45" s="51" t="n">
+      <c r="L45" s="49" t="n">
         <v>3019</v>
       </c>
       <c r="N45" s="0" t="n">
@@ -9901,4 +9898,117 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.65587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1.3599912378</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.9695279357</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4.6324322995</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.9242057955</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.6588596398</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3.1480502664</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1.0947733332</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.7804560062</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3.7290411943</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.8056102794</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.5743137526</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2.7440875909</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.2251413941</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.1605016745</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.7668816069</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>